<commit_message>
Correzione report-checklist.xlsx casi 44 e 54 colonna "Gestione errore"
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ARBITEKXXXX/Arbitek/XM-Lab/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111ARBITEKXXXX/Arbitek/XM-Lab/2.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sviluppo\azospvr\fser2.0\accreditamento\github\it-fse-accreditamento\GATEWAY\A1#111ARBITEKXXXX\Arbitek\XM-Lab\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ADA277-EC42-4380-A4F6-11C9211017AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9387D1-F824-4C21-9DBE-A1369BE997CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="38040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="198">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -756,9 +756,6 @@
     <t>f45614a925715f31</t>
   </si>
   <si>
-    <t>La procedura viene ritentata alla successiva schedulazione</t>
-  </si>
-  <si>
     <t>2023-04-11T10:05:25Z</t>
   </si>
   <si>
@@ -850,6 +847,12 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.50912.4.4.1.d6cc9a06ccb80f7ad04d4983bc37257f90e8ddc297a591258cb3fbd34c85814d.b086a4b332^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>La procedura viene ritentata alla successiva schedulazione. L'operazione è automatica senza intervento dell'utente</t>
+  </si>
+  <si>
+    <t>La procedura viene monitorata ed eventuali errori sono gestiti dal personale tecnico, che provvede a correggere la configurrazione o segnalare al personale clinico la non conformità del confidendialitycode per la correzione, a seconda dei cas (se dipendente da configurazione o se da modalità di refertazione)</t>
   </si>
 </sst>
 </file>
@@ -3758,10 +3761,10 @@
   <dimension ref="A1:T246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="M14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="O21" sqref="O21"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4323,7 +4326,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="45.75" thickBot="1">
+    <row r="17" spans="1:20" ht="75.75" thickBot="1">
       <c r="A17" s="20">
         <v>44</v>
       </c>
@@ -4352,13 +4355,15 @@
       <c r="L17" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="M17" s="25"/>
+      <c r="M17" s="33" t="s">
+        <v>161</v>
+      </c>
       <c r="N17" s="25"/>
       <c r="O17" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P17" s="33" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26" t="s">
@@ -4389,13 +4394,13 @@
         <v>45027</v>
       </c>
       <c r="G18" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="H18" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="I18" s="24" t="s">
         <v>167</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>168</v>
       </c>
       <c r="J18" s="33" t="s">
         <v>71</v>
@@ -4441,13 +4446,13 @@
         <v>45027</v>
       </c>
       <c r="G19" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="H19" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="I19" s="24" t="s">
         <v>170</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>171</v>
       </c>
       <c r="J19" s="33" t="s">
         <v>71</v>
@@ -4473,7 +4478,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="120.75" thickBot="1">
+    <row r="20" spans="1:20" ht="195.75" thickBot="1">
       <c r="A20" s="20">
         <v>54</v>
       </c>
@@ -4493,13 +4498,13 @@
         <v>45027</v>
       </c>
       <c r="G20" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="I20" s="24" t="s">
         <v>173</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>174</v>
       </c>
       <c r="J20" s="33" t="s">
         <v>71</v>
@@ -4516,7 +4521,7 @@
         <v>71</v>
       </c>
       <c r="P20" s="33" t="s">
-        <v>162</v>
+        <v>197</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
@@ -4549,7 +4554,7 @@
         <v>146</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L21" s="33"/>
       <c r="M21" s="33"/>
@@ -4583,13 +4588,13 @@
         <v>45027</v>
       </c>
       <c r="G22" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="H22" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="H22" s="24" t="s">
+      <c r="I22" s="24" t="s">
         <v>177</v>
-      </c>
-      <c r="I22" s="24" t="s">
-        <v>178</v>
       </c>
       <c r="J22" s="33" t="s">
         <v>71</v>
@@ -4635,13 +4640,13 @@
         <v>45027</v>
       </c>
       <c r="G23" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="H23" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="H23" s="24" t="s">
+      <c r="I23" s="24" t="s">
         <v>180</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>181</v>
       </c>
       <c r="J23" s="33" t="s">
         <v>71</v>
@@ -4687,13 +4692,13 @@
         <v>45027</v>
       </c>
       <c r="G24" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="H24" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="I24" s="24" t="s">
         <v>183</v>
-      </c>
-      <c r="H24" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>184</v>
       </c>
       <c r="J24" s="33" t="s">
         <v>71</v>
@@ -4739,13 +4744,13 @@
         <v>45027</v>
       </c>
       <c r="G25" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="I25" s="24" t="s">
         <v>186</v>
-      </c>
-      <c r="H25" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="I25" s="24" t="s">
-        <v>187</v>
       </c>
       <c r="J25" s="33" t="s">
         <v>71</v>
@@ -4791,13 +4796,13 @@
         <v>45027</v>
       </c>
       <c r="G26" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="H26" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="H26" s="24" t="s">
+      <c r="I26" s="24" t="s">
         <v>189</v>
-      </c>
-      <c r="I26" s="24" t="s">
-        <v>190</v>
       </c>
       <c r="J26" s="33" t="s">
         <v>71</v>
@@ -4843,13 +4848,13 @@
         <v>45027</v>
       </c>
       <c r="G27" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="H27" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="H27" s="24" t="s">
+      <c r="I27" s="24" t="s">
         <v>192</v>
-      </c>
-      <c r="I27" s="24" t="s">
-        <v>193</v>
       </c>
       <c r="J27" s="33" t="s">
         <v>71</v>
@@ -4895,13 +4900,13 @@
         <v>45027</v>
       </c>
       <c r="G28" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="H28" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="H28" s="24" t="s">
+      <c r="I28" s="24" t="s">
         <v>195</v>
-      </c>
-      <c r="I28" s="24" t="s">
-        <v>196</v>
       </c>
       <c r="J28" s="33" t="s">
         <v>71</v>

</xml_diff>